<commit_message>
Update of time report
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <workbookPr autoCompressPictures="0"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Namn</t>
   </si>
@@ -57,106 +63,88 @@
   </si>
   <si>
     <t>Getting the map to work properly. And also testing the database. Also added a few settings on the map.</t>
+  </si>
+  <si>
+    <t>Emailed all sections, sought out working logos, setup of project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="YYYY/MM/DD" numFmtId="165"/>
-    <numFmt formatCode="0.00" numFmtId="166"/>
-    <numFmt formatCode="@" numFmtId="167"/>
-  </numFmts>
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF4F6228"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF77933C"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF006100"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFCD5B5"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF4F6228"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFEBF1DE"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF254061"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF77933C"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFF2DCDB"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFFCD5B5"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFDCE6F2"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFEBF1DE"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF254061"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFF2DCDB"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFDCE6F2"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="10">
@@ -216,291 +204,232 @@
     </fill>
   </fills>
   <borders count="9">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thick"/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
-      <top style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="4" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="5" fontId="8" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="5" fontId="8" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="3" fontId="9" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="6" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="6" fontId="10" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="7" fontId="11" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="7" fontId="11" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="8" fontId="12" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="8" fontId="12" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="true" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="9" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="9" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="9" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="8" fillId="9" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="3" fontId="5" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="TableStyleLight1" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="1" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FFFDEADA"/>
         <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFB7DEE8"/>
-        <sz val="12"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FF254061"/>
+          <bgColor rgb="FFE46C0A"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FFD7E4BD"/>
         <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF77933C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <color rgb="FFF2DCDB"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF953735"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
         <color rgb="FF17375E"/>
-        <sz val="12"/>
+        <name val="Calibri"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF95B3D7"/>
@@ -509,50 +438,19 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="12"/>
+        <color rgb="FFB7DEE8"/>
         <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFF2DCDB"/>
-        <sz val="12"/>
       </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FF953735"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFD7E4BD"/>
-        <sz val="12"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF77933C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFDEADA"/>
-        <sz val="12"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE46C0A"/>
+          <bgColor rgb="FF254061"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -611,39 +509,361 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF254061"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AW15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A8" xSplit="0" ySplit="7"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="H20" activeCellId="0" pane="bottomLeft" sqref="H20"/>
+    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.62325581395349"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.12093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="3.50232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="7.62325581395349"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="7.13023255813954"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="167.995348837209"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="3.62790697674419"/>
-    <col collapsed="false" hidden="false" max="49" min="10" style="1" width="11"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="11"/>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="8.83203125" style="6"/>
+    <col min="9" max="9" width="8.83203125" style="7"/>
+    <col min="10" max="49" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1" s="12">
+    <row r="1" spans="1:49" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -698,13 +918,13 @@
       <c r="AV1" s="11"/>
       <c r="AW1" s="11"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2" s="22">
+    <row r="2" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="13"/>
       <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="n">
-        <f aca="false">SUMIF(G8:G998,"Fredrik",F8:F998)</f>
+      <c r="C2" s="15">
+        <f>SUMIF(G8:G998,"Fredrik",F8:F998)</f>
         <v>6</v>
       </c>
       <c r="D2" s="16"/>
@@ -754,13 +974,13 @@
       <c r="AV2" s="16"/>
       <c r="AW2" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3" s="22">
+    <row r="3" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24" t="n">
-        <f aca="false">SUMIF(G8:G998,"Niklas",F8:F998)</f>
+      <c r="C3" s="24">
+        <f>SUMIF(G8:G998,"Niklas",F8:F998)</f>
         <v>1</v>
       </c>
       <c r="D3" s="16"/>
@@ -810,13 +1030,13 @@
       <c r="AV3" s="16"/>
       <c r="AW3" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4" s="22">
+    <row r="4" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26" t="n">
-        <f aca="false">SUMIF(G8:G998,"Anders",F8:F998)</f>
+      <c r="C4" s="26">
+        <f>SUMIF(G8:G998,"Anders",F8:F998)</f>
         <v>3</v>
       </c>
       <c r="D4" s="16"/>
@@ -866,14 +1086,14 @@
       <c r="AV4" s="16"/>
       <c r="AW4" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5" s="22">
+    <row r="5" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="n">
-        <f aca="false">SUMIF(G8:G998,"Sofie",F8:F998)</f>
-        <v>1</v>
+      <c r="C5" s="28">
+        <f>SUMIF(G8:G998,"Sofie",F8:F998)</f>
+        <v>3</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="17"/>
@@ -922,13 +1142,13 @@
       <c r="AV5" s="16"/>
       <c r="AW5" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6" s="22">
+    <row r="6" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="30" t="n">
-        <f aca="false">SUMIF(G8:G998,"Rene",F8:F998)</f>
+      <c r="C6" s="30">
+        <f>SUMIF(G8:G998,"Rene",F8:F998)</f>
         <v>1</v>
       </c>
       <c r="D6" s="16"/>
@@ -978,7 +1198,7 @@
       <c r="AV6" s="16"/>
       <c r="AW6" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="17.25" outlineLevel="0" r="7" s="22">
+    <row r="7" spans="1:49" s="22" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1037,11 +1257,11 @@
       <c r="AV7" s="13"/>
       <c r="AW7" s="13"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
-      <c r="E8" s="37" t="n">
+    <row r="8" spans="1:49" ht="15" customHeight="1">
+      <c r="E8" s="37">
         <v>41354</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="4">
         <v>1</v>
       </c>
       <c r="G8" s="38" t="s">
@@ -1051,11 +1271,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="E9" s="37" t="n">
+    <row r="9" spans="1:49" ht="15" customHeight="1">
+      <c r="E9" s="37">
         <v>41354</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -1065,11 +1285,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
-      <c r="E10" s="37" t="n">
+    <row r="10" spans="1:49" ht="15" customHeight="1">
+      <c r="E10" s="37">
         <v>41354</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="38" t="s">
@@ -1079,11 +1299,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="E11" s="37" t="n">
+    <row r="11" spans="1:49" ht="15" customHeight="1">
+      <c r="E11" s="37">
         <v>41354</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="G11" s="38" t="s">
@@ -1093,11 +1313,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="E12" s="37" t="n">
+    <row r="12" spans="1:49" ht="15" customHeight="1">
+      <c r="E12" s="37">
         <v>41354</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -1107,11 +1327,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="E13" s="3" t="n">
+    <row r="13" spans="1:49" ht="15" customHeight="1">
+      <c r="E13" s="3">
         <v>41379</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4">
         <v>2</v>
       </c>
       <c r="G13" s="38" t="s">
@@ -1121,11 +1341,11 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="E14" s="3" t="n">
+    <row r="14" spans="1:49" ht="15" customHeight="1">
+      <c r="E14" s="3">
         <v>41379</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4">
         <v>2</v>
       </c>
       <c r="G14" s="38" t="s">
@@ -1135,11 +1355,11 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="E15" s="3" t="n">
+    <row r="15" spans="1:49" ht="15" customHeight="1">
+      <c r="E15" s="3">
         <v>41380</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4">
         <v>3</v>
       </c>
       <c r="G15" s="38" t="s">
@@ -1149,86 +1369,30 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="E15" s="3" t="n">
-        <v>41380</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="38" t="s">
+    <row r="16" spans="1:49" ht="15" customHeight="1">
+      <c r="E16" s="3">
+        <v>41381</v>
+      </c>
+      <c r="F16" s="4">
         <v>2</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="E15" s="3" t="n">
-        <v>41380</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="E15" s="3" t="n">
-        <v>41380</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="E15" s="3" t="n">
-        <v>41380</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
+      <c r="G16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="19" ht="15" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="G1:G7;G95:G1048576">
-    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="equal" percent="0" priority="2" rank="0" text="" type="cellIs">
-      <formula>"Maria"</formula>
-    </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="1" operator="equal" percent="0" priority="3" rank="0" text="" type="cellIs">
-      <formula>"Rickard"</formula>
-    </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="2" operator="equal" percent="0" priority="4" rank="0" text="" type="cellIs">
-      <formula>"Sofie"</formula>
-    </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="3" operator="equal" percent="0" priority="5" rank="0" text="" type="cellIs">
-      <formula>"Niklas"</formula>
-    </cfRule>
-    <cfRule aboveAverage="0" bottom="0" dxfId="4" operator="equal" percent="0" priority="6" rank="0" text="" type="cellIs">
-      <formula>"Simon"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolving a few errors
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Namn</t>
   </si>
@@ -75,17 +75,24 @@
   </si>
   <si>
     <t>Research on fancy menu but ended with implemented basic one.</t>
+  </si>
+  <si>
+    <t>Meeting and coding</t>
+  </si>
+  <si>
+    <t>Database and learning and implementing unittests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="YYYY/MM/DD" numFmtId="165"/>
     <numFmt formatCode="0.00" numFmtId="166"/>
     <numFmt formatCode="@" numFmtId="167"/>
+    <numFmt formatCode="YYYY/MM/DD" numFmtId="168"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -327,7 +334,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -486,6 +493,10 @@
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -496,7 +507,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="TableStyleLight1" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in TableStyleLight1" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -566,10 +577,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AW24"/>
+  <dimension ref="A1:AW26"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="H27" activeCellId="0" pane="topLeft" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -582,6 +593,7 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="6" width="8.87906976744186"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="8.87906976744186"/>
     <col collapsed="false" hidden="false" max="49" min="10" style="1" width="8.87906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.66511627906977"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1" s="12">
@@ -646,7 +658,7 @@
       </c>
       <c r="C2" s="15" t="n">
         <f aca="false">SUMIF(G8:G998,"Fredrik",F8:F998)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
@@ -1216,6 +1228,34 @@
         <v>19</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="25">
+      <c r="E25" s="40" t="n">
+        <v>41383</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="26">
+      <c r="E26" s="3" t="n">
+        <v>41384</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added a menu system with a bottom bar, aswell as added a layers feature.
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Namn</t>
   </si>
@@ -84,106 +83,100 @@
   </si>
   <si>
     <t>Coding querys</t>
+  </si>
+  <si>
+    <t>App logo and reading up on design</t>
+  </si>
+  <si>
+    <t>Looking over some work and reading on design</t>
+  </si>
+  <si>
+    <t>Implementing menu system and reading up on search interfaces</t>
+  </si>
+  <si>
+    <t>2013-14-16</t>
+  </si>
+  <si>
+    <t>Reading up on android, setting up system so forth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="YYYY/MM/DD" numFmtId="165"/>
-    <numFmt formatCode="0.00" numFmtId="166"/>
-    <numFmt formatCode="@" numFmtId="167"/>
-  </numFmts>
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF4F6228"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF77933C"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF006100"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFCD5B5"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF4F6228"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFEBF1DE"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF254061"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF77933C"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFF2DCDB"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFFCD5B5"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFDCE6F2"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFEBF1DE"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF254061"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFF2DCDB"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFDCE6F2"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="10">
@@ -243,270 +236,188 @@
     </fill>
   </fills>
   <borders count="9">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thick"/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
-      <top style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
-      <right style="thick"/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="4" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="5" fontId="8" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="5" fontId="8" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="3" fontId="9" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="9" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="6" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="6" fontId="10" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="7" fontId="11" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="7" fontId="11" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="8" fontId="12" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="8" fontId="12" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="true" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="9" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="9" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="9" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="8" fillId="9" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="3" fontId="5" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in TableStyleLight1" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -565,36 +476,331 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF254061"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AW27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW31"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E28" activeCellId="0" pane="topLeft" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="49" min="10" style="1" width="8.87906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.66511627906977"/>
+    <col min="1" max="3" width="8.875" style="1"/>
+    <col min="4" max="4" width="8.875" style="2"/>
+    <col min="5" max="5" width="10.5" style="3"/>
+    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="7" max="7" width="8.875" style="5"/>
+    <col min="8" max="8" width="8.875" style="6"/>
+    <col min="9" max="9" width="8.875" style="7"/>
+    <col min="10" max="49" width="8.875" style="1"/>
+    <col min="50" max="1025" width="8.625"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1" s="12">
+    <row r="1" spans="1:49" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -649,13 +855,13 @@
       <c r="AV1" s="11"/>
       <c r="AW1" s="11"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2" s="22">
+    <row r="2" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="n">
-        <f aca="false">SUMIF(G8:G998,"Fredrik",F8:F998)</f>
+      <c r="C2" s="15">
+        <f>SUMIF(G8:G998,"Fredrik",F8:F998)</f>
         <v>21</v>
       </c>
       <c r="D2" s="16"/>
@@ -705,14 +911,14 @@
       <c r="AV2" s="16"/>
       <c r="AW2" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3" s="22">
+    <row r="3" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24" t="n">
-        <f aca="false">SUMIF(G8:G998,"Niklas",F8:F998)</f>
-        <v>2</v>
+      <c r="C3" s="24">
+        <f>SUMIF(G8:G998,"Niklas",F8:F998)</f>
+        <v>10.5</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17"/>
@@ -761,13 +967,13 @@
       <c r="AV3" s="16"/>
       <c r="AW3" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4" s="22">
+    <row r="4" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26" t="n">
-        <f aca="false">SUMIF(G8:G998,"Anders",F8:F998)</f>
+      <c r="C4" s="26">
+        <f>SUMIF(G8:G998,"Anders",F8:F998)</f>
         <v>10</v>
       </c>
       <c r="D4" s="16"/>
@@ -817,13 +1023,13 @@
       <c r="AV4" s="16"/>
       <c r="AW4" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5" s="22">
+    <row r="5" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="n">
-        <f aca="false">SUMIF(G8:G998,"Sofie",F8:F998)</f>
+      <c r="C5" s="28">
+        <f>SUMIF(G8:G998,"Sofie",F8:F998)</f>
         <v>3</v>
       </c>
       <c r="D5" s="16"/>
@@ -873,13 +1079,13 @@
       <c r="AV5" s="16"/>
       <c r="AW5" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6" s="22">
+    <row r="6" spans="1:49" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="30" t="n">
-        <f aca="false">SUMIF(G8:G998,"Rene",F8:F998)</f>
+      <c r="C6" s="30">
+        <f>SUMIF(G8:G998,"Rene",F8:F998)</f>
         <v>2</v>
       </c>
       <c r="D6" s="16"/>
@@ -929,7 +1135,7 @@
       <c r="AV6" s="16"/>
       <c r="AW6" s="16"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="17.25" outlineLevel="0" r="7" s="22">
+    <row r="7" spans="1:49" s="22" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -988,11 +1194,11 @@
       <c r="AV7" s="13"/>
       <c r="AW7" s="13"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
-      <c r="E8" s="37" t="n">
+    <row r="8" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="37">
         <v>41354</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="4">
         <v>1</v>
       </c>
       <c r="G8" s="38" t="s">
@@ -1002,11 +1208,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="E9" s="37" t="n">
+    <row r="9" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="37">
         <v>41354</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="38" t="s">
@@ -1016,11 +1222,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
-      <c r="E10" s="37" t="n">
+    <row r="10" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="37">
         <v>41354</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="38" t="s">
@@ -1030,11 +1236,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="E11" s="37" t="n">
+    <row r="11" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="37">
         <v>41354</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="G11" s="38" t="s">
@@ -1044,11 +1250,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="E12" s="37" t="n">
+    <row r="12" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="37">
         <v>41354</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="38" t="s">
@@ -1058,11 +1264,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="E13" s="3" t="n">
+    <row r="13" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
         <v>41379</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4">
         <v>2</v>
       </c>
       <c r="G13" s="38" t="s">
@@ -1072,11 +1278,11 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="E14" s="3" t="n">
+    <row r="14" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
         <v>41379</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4">
         <v>2</v>
       </c>
       <c r="G14" s="38" t="s">
@@ -1086,11 +1292,11 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="E15" s="3" t="n">
+    <row r="15" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
         <v>41380</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4">
         <v>3</v>
       </c>
       <c r="G15" s="38" t="s">
@@ -1100,11 +1306,11 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="E16" s="3" t="n">
+    <row r="16" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="3">
         <v>41381</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="4">
         <v>2</v>
       </c>
       <c r="G16" s="38" t="s">
@@ -1114,11 +1320,11 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="E17" s="3" t="n">
+    <row r="17" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
         <v>41381</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="4">
         <v>3</v>
       </c>
       <c r="G17" s="38" t="s">
@@ -1128,11 +1334,11 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="E18" s="3" t="n">
+    <row r="18" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="3">
         <v>41379</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="4">
         <v>1</v>
       </c>
       <c r="G18" s="38" t="s">
@@ -1142,11 +1348,11 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="E19" s="3" t="n">
+    <row r="19" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
         <v>41379</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="4">
         <v>1</v>
       </c>
       <c r="G19" s="38" t="s">
@@ -1156,11 +1362,11 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="20">
-      <c r="E20" s="3" t="n">
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
         <v>41379</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="4">
         <v>1</v>
       </c>
       <c r="G20" s="38" t="s">
@@ -1170,11 +1376,11 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="21">
-      <c r="E21" s="3" t="n">
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="3">
         <v>41379</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="4">
         <v>1</v>
       </c>
       <c r="G21" s="38" t="s">
@@ -1184,11 +1390,11 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="22">
-      <c r="E22" s="3" t="n">
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="3">
         <v>41378</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="4">
         <v>1</v>
       </c>
       <c r="G22" s="38" t="s">
@@ -1198,11 +1404,11 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="23">
-      <c r="E23" s="3" t="n">
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E23" s="3">
         <v>41382</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="4">
         <v>2</v>
       </c>
       <c r="G23" s="38" t="s">
@@ -1212,11 +1418,11 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="24">
-      <c r="E24" s="3" t="n">
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="3">
         <v>41382</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="4">
         <v>4</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -1226,11 +1432,11 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="25">
-      <c r="E25" s="3" t="n">
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="3">
         <v>41383</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="4">
         <v>2</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -1240,11 +1446,11 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="26">
-      <c r="E26" s="3" t="n">
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="3">
         <v>41384</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="4">
         <v>4</v>
       </c>
       <c r="G26" s="5" t="s">
@@ -1254,11 +1460,11 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="27">
-      <c r="E27" s="3" t="n">
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="3">
         <v>41387</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="4">
         <v>4</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -1268,13 +1474,64 @@
         <v>22</v>
       </c>
     </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="3">
+        <v>41383</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="3">
+        <v>41387</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E30" s="3">
+        <v>41388</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="4">
+        <v>2</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added My location function and changed starting point
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16770" windowHeight="5115" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16440" windowHeight="6975" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="39">
   <si>
     <t>Namn</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Meeting 2 with Supervisor Max</t>
+  </si>
+  <si>
+    <t>meeting</t>
   </si>
 </sst>
 </file>
@@ -818,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW53"/>
+  <dimension ref="A1:AW59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -899,7 +902,7 @@
       </c>
       <c r="C2" s="16">
         <f>SUMIF(G8:G997,"Fredrik",F8:F997)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
@@ -955,7 +958,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUMIF(G8:G997,"Niklas",F8:F997)</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -1011,7 +1014,7 @@
       </c>
       <c r="C4" s="27">
         <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
@@ -1067,7 +1070,7 @@
       </c>
       <c r="C5" s="29">
         <f>SUMIF(G8:G997,"Sofie",F8:F997)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="18"/>
@@ -1123,7 +1126,7 @@
       </c>
       <c r="C6" s="31">
         <f>SUMIF(G8:G997,"Rene",F8:F997)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18"/>
@@ -1875,6 +1878,79 @@
         <v>37</v>
       </c>
     </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E54" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F54" s="4">
+        <v>1</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E55" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E56" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F56" s="4">
+        <v>1</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E57" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E58" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F58" s="4">
+        <v>1</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Now possible to draw a red line between two markers
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23115" windowHeight="7140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15150" windowHeight="7515" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="43">
   <si>
     <t>Namn</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Learned GUI-tests and added one.</t>
+  </si>
+  <si>
+    <t>Meeting 3 with Max</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,7 +627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -833,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW61"/>
+  <dimension ref="A1:AW64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -914,7 +917,7 @@
       </c>
       <c r="C2" s="16">
         <f>SUMIF(G8:G997,"Fredrik",F8:F997)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
@@ -1026,7 +1029,7 @@
       </c>
       <c r="C4" s="27">
         <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
@@ -1138,7 +1141,7 @@
       </c>
       <c r="C6" s="31">
         <f>SUMIF(G8:G997,"Rene",F8:F997)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18"/>
@@ -2002,6 +2005,48 @@
         <v>41</v>
       </c>
     </row>
+    <row r="62" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E62" s="3">
+        <v>41397</v>
+      </c>
+      <c r="F62" s="4">
+        <v>1</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E63" s="3">
+        <v>41397</v>
+      </c>
+      <c r="F63" s="4">
+        <v>1</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E64" s="3">
+        <v>41397</v>
+      </c>
+      <c r="F64" s="4">
+        <v>1</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Display duration and distance when walking. Draw a line between given points. Modified a little bit in the layout
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="6015" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20010" windowHeight="6120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
   <si>
     <t>Namn</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Beginning of paths through buildings</t>
+  </si>
+  <si>
+    <t>Draw path, get distance, get duration, modified layout.</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,7 +633,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW65"/>
+  <dimension ref="A1:AW66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1035,7 @@
       </c>
       <c r="C4" s="27">
         <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
@@ -2064,6 +2067,20 @@
         <v>43</v>
       </c>
     </row>
+    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E66" s="3">
+        <v>41399</v>
+      </c>
+      <c r="F66" s="4">
+        <v>7</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Scale for Rene to add markers
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20010" windowHeight="6120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16980" windowHeight="5580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="46">
   <si>
     <t>Namn</t>
   </si>
@@ -149,7 +149,10 @@
     <t>Beginning of paths through buildings</t>
   </si>
   <si>
-    <t>Draw path, get distance, get duration, modified layout.</t>
+    <t>Draw path, modified layout, draw line, JSON Parser</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Started to parse with ASyncTask distance, duration</t>
   </si>
 </sst>
 </file>
@@ -842,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW66"/>
+  <dimension ref="A1:AW67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1038,7 @@
       </c>
       <c r="C4" s="27">
         <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
@@ -2081,6 +2084,20 @@
         <v>44</v>
       </c>
     </row>
+    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E67" s="3">
+        <v>41399</v>
+      </c>
+      <c r="F67" s="4">
+        <v>3</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Kom på att jag varit dålig på att fylla i denna, men kommer vara bättre på det framöver
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="51">
   <si>
     <t>Namn</t>
   </si>
@@ -162,6 +161,12 @@
   </si>
   <si>
     <t>Error fixing</t>
+  </si>
+  <si>
+    <t>Redid all pivotal to userstories with tasks</t>
+  </si>
+  <si>
+    <t>Read up on menu systems, started working on some logos, reimplemented menu for showing lecturehalls</t>
   </si>
 </sst>
 </file>
@@ -854,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW78"/>
+  <dimension ref="A1:AW80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -934,7 +939,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="16">
-        <f>SUMIF(G8:G997,"Fredrik",F8:F997)</f>
+        <f>SUMIF(G8:G999,"Fredrik",F8:F999)</f>
         <v>51</v>
       </c>
       <c r="D2" s="17"/>
@@ -990,8 +995,8 @@
         <v>3</v>
       </c>
       <c r="C3" s="25">
-        <f>SUMIF(G8:G997,"Niklas",F8:F997)</f>
-        <v>18.5</v>
+        <f>SUMIF(G8:G999,"Niklas",F8:F999)</f>
+        <v>25.5</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -1046,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="27">
-        <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
+        <f>SUMIF(G8:G999,"Anders",F8:F999)</f>
         <v>32.5</v>
       </c>
       <c r="D4" s="17"/>
@@ -1102,7 +1107,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="29">
-        <f>SUMIF(G8:G997,"Sofie",F8:F997)</f>
+        <f>SUMIF(G8:G999,"Sofie",F8:F999)</f>
         <v>8</v>
       </c>
       <c r="D5" s="17"/>
@@ -1158,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="31">
-        <f>SUMIF(G8:G997,"Rene",F8:F997)</f>
+        <f>SUMIF(G8:G999,"Rene",F8:F999)</f>
         <v>27</v>
       </c>
       <c r="D6" s="17"/>
@@ -2081,16 +2086,16 @@
     </row>
     <row r="66" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E66" s="3">
-        <v>41399</v>
+        <v>41397</v>
       </c>
       <c r="F66" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="5:8" x14ac:dyDescent="0.25">
@@ -2098,27 +2103,27 @@
         <v>41399</v>
       </c>
       <c r="F67" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E68" s="3">
-        <v>41400</v>
+        <v>41399</v>
       </c>
       <c r="F68" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="5:8" x14ac:dyDescent="0.25">
@@ -2129,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>46</v>
@@ -2143,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>46</v>
@@ -2157,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>46</v>
@@ -2171,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>46</v>
@@ -2179,16 +2184,16 @@
     </row>
     <row r="73" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E73" s="3">
-        <v>41407</v>
+        <v>41400</v>
       </c>
       <c r="F73" s="4">
         <v>1</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="5:8" x14ac:dyDescent="0.25">
@@ -2199,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>47</v>
@@ -2213,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>47</v>
@@ -2227,7 +2232,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>47</v>
@@ -2241,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>47</v>
@@ -2252,13 +2257,41 @@
         <v>41407</v>
       </c>
       <c r="F78" s="4">
+        <v>1</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E79" s="3">
+        <v>41407</v>
+      </c>
+      <c r="F79" s="4">
         <v>0.5</v>
       </c>
-      <c r="G78" s="5" t="s">
+      <c r="G79" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="H79" s="6" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E80" s="3">
+        <v>41407</v>
+      </c>
+      <c r="F80" s="4">
+        <v>5</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arbetsdagboken updated again :)
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="51">
   <si>
     <t>Namn</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Draw path, modified layout, draw line, JSON Parser</t>
   </si>
   <si>
-    <t xml:space="preserve"> Started to parse with ASyncTask distance, duration</t>
-  </si>
-  <si>
     <t>Regular Monday meeting</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t>Review of documentation</t>
+  </si>
+  <si>
+    <t>Started to parse with ASyncTask distance, duration</t>
+  </si>
+  <si>
+    <t>Get distance without drawing(not working without async)</t>
   </si>
 </sst>
 </file>
@@ -857,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW79"/>
+  <dimension ref="A1:AW80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="B70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1053,7 @@
       </c>
       <c r="C4" s="27">
         <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
@@ -2107,7 +2110,7 @@
         <v>4</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" spans="5:8" x14ac:dyDescent="0.25">
@@ -2121,7 +2124,7 @@
         <v>4</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="5:8" x14ac:dyDescent="0.25">
@@ -2135,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="5:8" x14ac:dyDescent="0.25">
@@ -2149,7 +2152,7 @@
         <v>6</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="5:8" x14ac:dyDescent="0.25">
@@ -2163,7 +2166,7 @@
         <v>5</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="5:8" x14ac:dyDescent="0.25">
@@ -2177,7 +2180,7 @@
         <v>3</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="5:8" x14ac:dyDescent="0.25">
@@ -2191,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="5:8" x14ac:dyDescent="0.25">
@@ -2205,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="5:8" x14ac:dyDescent="0.25">
@@ -2219,7 +2222,7 @@
         <v>6</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="5:8" x14ac:dyDescent="0.25">
@@ -2233,7 +2236,7 @@
         <v>5</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="5:8" x14ac:dyDescent="0.25">
@@ -2247,7 +2250,7 @@
         <v>3</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="5:8" x14ac:dyDescent="0.25">
@@ -2261,7 +2264,7 @@
         <v>4</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="5:8" x14ac:dyDescent="0.25">
@@ -2275,7 +2278,21 @@
         <v>4</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E80" s="3">
+        <v>41402</v>
+      </c>
+      <c r="F80" s="4">
+        <v>3</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch mode bug fix
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16770" windowHeight="6735" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16770" windowHeight="8580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="53">
   <si>
     <t>Namn</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Get distance without drawing(not working without async)</t>
+  </si>
+  <si>
+    <t>Exit function and simplied navigation for first version release</t>
+  </si>
+  <si>
+    <t>Bug fix: switch mode</t>
   </si>
 </sst>
 </file>
@@ -860,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW80"/>
+  <dimension ref="A1:AW82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView tabSelected="1" topLeftCell="B64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1059,7 @@
       </c>
       <c r="C4" s="27">
         <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
@@ -2295,6 +2301,34 @@
         <v>50</v>
       </c>
     </row>
+    <row r="81" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E81" s="3">
+        <v>41407</v>
+      </c>
+      <c r="F81" s="4">
+        <v>2</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E82" s="3">
+        <v>41407</v>
+      </c>
+      <c r="F82" s="4">
+        <v>1</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Removed the option to switch mode
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="54">
   <si>
     <t>Namn</t>
   </si>
@@ -174,6 +173,9 @@
   </si>
   <si>
     <t>Bug fix: switch mode</t>
+  </si>
+  <si>
+    <t>Working some with the UI, reading up on how to switch mode, and also designed a daymode and nighmode logo, and then realising it shouldnt even be two modes :P</t>
   </si>
 </sst>
 </file>
@@ -866,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW82"/>
+  <dimension ref="A1:AW83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1005,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUMIF(G8:G997,"Niklas",F8:F997)</f>
-        <v>18.5</v>
+        <v>21.5</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -2329,6 +2331,20 @@
         <v>52</v>
       </c>
     </row>
+    <row r="83" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E83" s="3">
+        <v>41408</v>
+      </c>
+      <c r="F83" s="4">
+        <v>3</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
ICal reader, not yet fully functional
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="58">
   <si>
     <t>Namn</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>Working some with the UI, reading up on how to switch mode, and also designed a daymode and nighmode logo, and then realising it shouldnt even be two modes :P</t>
+  </si>
+  <si>
+    <t>Continue working on the custom snippets, also looking in to a custom layers selection</t>
+  </si>
+  <si>
+    <t>Working with the custom snippets, and a simple steptracker</t>
+  </si>
+  <si>
+    <t>Refined the steptracker to one that actually works, refactored some code</t>
+  </si>
+  <si>
+    <t>Started working on iCal synchronization</t>
   </si>
 </sst>
 </file>
@@ -868,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW83"/>
+  <dimension ref="A1:AW87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1017,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUMIF(G8:G997,"Niklas",F8:F997)</f>
-        <v>21.5</v>
+        <v>34</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -2345,6 +2357,62 @@
         <v>53</v>
       </c>
     </row>
+    <row r="84" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E84" s="3">
+        <v>41409</v>
+      </c>
+      <c r="F84" s="4">
+        <v>4</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E85" s="3">
+        <v>41410</v>
+      </c>
+      <c r="F85" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E86" s="3">
+        <v>41411</v>
+      </c>
+      <c r="F86" s="4">
+        <v>2</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E87" s="3">
+        <v>41412</v>
+      </c>
+      <c r="F87" s="4">
+        <v>4</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Removed old doc. Added three new in Release doc folder.
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16770" windowHeight="8580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="30980" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="62">
   <si>
     <t>Namn</t>
   </si>
@@ -188,13 +193,25 @@
   </si>
   <si>
     <t>Started working on iCal synchronization</t>
+  </si>
+  <si>
+    <t>Mailing, researching documentation</t>
+  </si>
+  <si>
+    <t>Looking up and setting up gitHub and Eclipse with help of friend</t>
+  </si>
+  <si>
+    <t>Structuring documentation</t>
+  </si>
+  <si>
+    <t>Went through lecture info, reasearched internet, other course docs, Max instructions etc. and setup User Manual, Developer Manual and Software Dev Document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -266,8 +283,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,12 +317,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF77933C"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFEBF1DE"/>
       </patternFill>
     </fill>
     <fill>
@@ -326,6 +353,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD7E4BD"/>
         <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor rgb="FFEBF1DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FFEBF1DE"/>
       </patternFill>
     </fill>
   </fills>
@@ -424,9 +463,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -446,22 +499,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -475,40 +522,60 @@
     <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="16">
+    <cellStyle name="Följd hyperlänk" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -880,26 +947,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW87"/>
+  <dimension ref="A1:AW91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="8.75" style="1"/>
-    <col min="4" max="4" width="8.75" style="2"/>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
     <col min="5" max="5" width="10.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.75" style="4"/>
-    <col min="7" max="7" width="8.75" style="5"/>
-    <col min="8" max="8" width="72.875" style="6"/>
-    <col min="9" max="9" width="8.75" style="7"/>
-    <col min="10" max="49" width="8.75" style="1"/>
-    <col min="50" max="1025" width="8.75"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="136.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="7"/>
+    <col min="10" max="49" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -908,350 +974,350 @@
         <v>1</v>
       </c>
       <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-    </row>
-    <row r="2" spans="1:49" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="16">
-        <f>SUMIF(G8:G997,"Fredrik",F8:F997)</f>
+      <c r="E1" s="37"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+    </row>
+    <row r="2" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15">
+        <f>SUMIF(G9:G1000,"Fredrik",F9:F1000)</f>
         <v>51</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="17"/>
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
-      <c r="AL2" s="17"/>
-      <c r="AM2" s="17"/>
-      <c r="AN2" s="17"/>
-      <c r="AO2" s="17"/>
-      <c r="AP2" s="17"/>
-      <c r="AQ2" s="17"/>
-      <c r="AR2" s="17"/>
-      <c r="AS2" s="17"/>
-      <c r="AT2" s="17"/>
-      <c r="AU2" s="17"/>
-      <c r="AV2" s="17"/>
-      <c r="AW2" s="17"/>
-    </row>
-    <row r="3" spans="1:49" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="24" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="16"/>
+      <c r="AO2" s="16"/>
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="16"/>
+      <c r="AR2" s="16"/>
+      <c r="AS2" s="16"/>
+      <c r="AT2" s="16"/>
+      <c r="AU2" s="16"/>
+      <c r="AV2" s="16"/>
+      <c r="AW2" s="16"/>
+    </row>
+    <row r="3" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="25">
-        <f>SUMIF(G8:G997,"Niklas",F8:F997)</f>
+      <c r="C3" s="23">
+        <f>SUMIF(G9:G1000,"Niklas",F9:F1000)</f>
         <v>34</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17"/>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="17"/>
-      <c r="AM3" s="17"/>
-      <c r="AN3" s="17"/>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="17"/>
-      <c r="AR3" s="17"/>
-      <c r="AS3" s="17"/>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="17"/>
-      <c r="AV3" s="17"/>
-      <c r="AW3" s="17"/>
-    </row>
-    <row r="4" spans="1:49" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="27">
-        <f>SUMIF(G8:G997,"Anders",F8:F997)</f>
+      <c r="D3" s="16"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="16"/>
+    </row>
+    <row r="4" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="25">
+        <f>SUMIF(G9:G1000,"Anders",F9:F1000)</f>
         <v>39</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="17"/>
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
-      <c r="AL4" s="17"/>
-      <c r="AM4" s="17"/>
-      <c r="AN4" s="17"/>
-      <c r="AO4" s="17"/>
-      <c r="AP4" s="17"/>
-      <c r="AQ4" s="17"/>
-      <c r="AR4" s="17"/>
-      <c r="AS4" s="17"/>
-      <c r="AT4" s="17"/>
-      <c r="AU4" s="17"/>
-      <c r="AV4" s="17"/>
-      <c r="AW4" s="17"/>
-    </row>
-    <row r="5" spans="1:49" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="28" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
+      <c r="AQ4" s="16"/>
+      <c r="AR4" s="16"/>
+      <c r="AS4" s="16"/>
+      <c r="AT4" s="16"/>
+      <c r="AU4" s="16"/>
+      <c r="AV4" s="16"/>
+      <c r="AW4" s="16"/>
+    </row>
+    <row r="5" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="13"/>
+      <c r="B5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="29">
-        <f>SUMIF(G8:G997,"Sofie",F8:F997)</f>
+      <c r="C5" s="27">
+        <f>SUMIF(G9:G1000,"Sofie",F8:F1000)</f>
+        <v>23</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="16"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="16"/>
+      <c r="AP5" s="16"/>
+      <c r="AQ5" s="16"/>
+      <c r="AR5" s="16"/>
+      <c r="AS5" s="16"/>
+      <c r="AT5" s="16"/>
+      <c r="AU5" s="16"/>
+      <c r="AV5" s="16"/>
+      <c r="AW5" s="16"/>
+    </row>
+    <row r="6" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="13"/>
+      <c r="B6" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="29">
+        <f>SUMIF(G9:G1000,"Rene",F9:F1000)</f>
+        <v>27</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="16"/>
+      <c r="AO6" s="16"/>
+      <c r="AP6" s="16"/>
+      <c r="AQ6" s="16"/>
+      <c r="AR6" s="16"/>
+      <c r="AS6" s="16"/>
+      <c r="AT6" s="16"/>
+      <c r="AU6" s="16"/>
+      <c r="AV6" s="16"/>
+      <c r="AW6" s="16"/>
+    </row>
+    <row r="7" spans="1:49" s="21" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="17"/>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="17"/>
-      <c r="AH5" s="17"/>
-      <c r="AI5" s="17"/>
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
-      <c r="AL5" s="17"/>
-      <c r="AM5" s="17"/>
-      <c r="AN5" s="17"/>
-      <c r="AO5" s="17"/>
-      <c r="AP5" s="17"/>
-      <c r="AQ5" s="17"/>
-      <c r="AR5" s="17"/>
-      <c r="AS5" s="17"/>
-      <c r="AT5" s="17"/>
-      <c r="AU5" s="17"/>
-      <c r="AV5" s="17"/>
-      <c r="AW5" s="17"/>
-    </row>
-    <row r="6" spans="1:49" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="31">
-        <f>SUMIF(G8:G997,"Rene",F8:F997)</f>
-        <v>27</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="17"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="17"/>
-      <c r="AG6" s="17"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="17"/>
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="17"/>
-      <c r="AM6" s="17"/>
-      <c r="AN6" s="17"/>
-      <c r="AO6" s="17"/>
-      <c r="AP6" s="17"/>
-      <c r="AQ6" s="17"/>
-      <c r="AR6" s="17"/>
-      <c r="AS6" s="17"/>
-      <c r="AT6" s="17"/>
-      <c r="AU6" s="17"/>
-      <c r="AV6" s="17"/>
-      <c r="AW6" s="17"/>
-    </row>
-    <row r="7" spans="1:49" s="23" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="37"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
@@ -1282,564 +1348,564 @@
       <c r="AK7" s="8"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8"/>
-      <c r="AN7" s="14"/>
-      <c r="AO7" s="14"/>
-      <c r="AP7" s="14"/>
-      <c r="AQ7" s="14"/>
-      <c r="AR7" s="14"/>
-      <c r="AS7" s="14"/>
-      <c r="AT7" s="14"/>
-      <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="14"/>
-    </row>
-    <row r="8" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+    </row>
+    <row r="8" spans="1:49" ht="15" customHeight="1">
       <c r="E8" s="3">
-        <v>41354</v>
+        <v>41352</v>
       </c>
       <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" ht="15" customHeight="1">
       <c r="E9" s="3">
         <v>41354</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="39" t="s">
+      <c r="G9" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" ht="15" customHeight="1">
       <c r="E10" s="3">
         <v>41354</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="39" t="s">
+      <c r="G10" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" ht="15" customHeight="1">
       <c r="E11" s="3">
         <v>41354</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="39" t="s">
+      <c r="G11" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" ht="15" customHeight="1">
       <c r="E12" s="3">
         <v>41354</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="39" t="s">
+      <c r="G12" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" ht="15" customHeight="1">
       <c r="E13" s="3">
-        <v>41379</v>
+        <v>41354</v>
       </c>
       <c r="F13" s="4">
-        <v>2</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" ht="15" customHeight="1">
       <c r="E14" s="3">
         <v>41379</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
       </c>
-      <c r="G14" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="39" t="s">
+      <c r="G14" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" ht="15" customHeight="1">
+      <c r="E15" s="3">
+        <v>41379</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="3">
+    <row r="16" spans="1:49" ht="15" customHeight="1">
+      <c r="E16" s="3">
         <v>41380</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F16" s="4">
         <v>3</v>
       </c>
-      <c r="G15" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="39" t="s">
+      <c r="G16" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="3">
-        <v>41381</v>
-      </c>
-      <c r="F16" s="4">
-        <v>2</v>
-      </c>
-      <c r="G16" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:8" ht="15" customHeight="1">
       <c r="E17" s="3">
         <v>41381</v>
       </c>
       <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" ht="15" customHeight="1">
+      <c r="E18" s="3">
+        <v>41381</v>
+      </c>
+      <c r="F18" s="4">
         <v>3</v>
       </c>
-      <c r="G17" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="39" t="s">
+      <c r="G18" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="3">
-        <v>41379</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:8" ht="15" customHeight="1">
       <c r="E19" s="3">
         <v>41379</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="G19" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="39" t="s">
+      <c r="G19" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:8" ht="15" customHeight="1">
       <c r="E20" s="3">
         <v>41379</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="39" t="s">
+      <c r="G20" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:8">
       <c r="E21" s="3">
         <v>41379</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="39" t="s">
+      <c r="G21" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:8">
       <c r="E22" s="3">
+        <v>41379</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8">
+      <c r="E23" s="3">
         <v>41378</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="39" t="s">
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E23" s="3">
-        <v>41382</v>
-      </c>
-      <c r="F23" s="4">
-        <v>2</v>
-      </c>
-      <c r="G23" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:8">
       <c r="E24" s="3">
         <v>41382</v>
       </c>
       <c r="F24" s="4">
-        <v>4</v>
-      </c>
-      <c r="G24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8">
+      <c r="E25" s="3">
+        <v>41382</v>
+      </c>
+      <c r="F25" s="4">
+        <v>4</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="3">
+    <row r="26" spans="5:8">
+      <c r="E26" s="3">
         <v>41383</v>
       </c>
-      <c r="F25" s="4">
-        <v>2</v>
-      </c>
-      <c r="G25" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="39" t="s">
+      <c r="F26" s="4">
+        <v>2</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="3">
+    <row r="27" spans="5:8">
+      <c r="E27" s="3">
         <v>41384</v>
       </c>
-      <c r="F26" s="4">
-        <v>4</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="39" t="s">
+      <c r="F27" s="4">
+        <v>4</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="36" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="3">
+    <row r="28" spans="5:8">
+      <c r="E28" s="3">
         <v>41387</v>
       </c>
-      <c r="F27" s="4">
-        <v>4</v>
-      </c>
-      <c r="G27" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27" s="39" t="s">
+      <c r="F28" s="4">
+        <v>4</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E28" s="3">
+    <row r="29" spans="5:8">
+      <c r="E29" s="3">
         <v>41383</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F29" s="4">
         <v>3</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G29" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="39" t="s">
+      <c r="H29" s="36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E29" s="3">
+    <row r="30" spans="5:8">
+      <c r="E30" s="3">
         <v>41387</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F30" s="4">
         <v>0.5</v>
       </c>
-      <c r="G29" s="38" t="s">
+      <c r="G30" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="39" t="s">
+      <c r="H30" s="36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E30" s="3">
+    <row r="31" spans="5:8">
+      <c r="E31" s="3">
         <v>41388</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F31" s="4">
         <v>3</v>
       </c>
-      <c r="G30" s="38" t="s">
+      <c r="G31" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="H31" s="36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E31" s="3">
-        <v>41380</v>
-      </c>
-      <c r="F31" s="4">
-        <v>2</v>
-      </c>
-      <c r="G31" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:8">
       <c r="E32" s="3">
         <v>41380</v>
       </c>
       <c r="F32" s="4">
+        <v>2</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8">
+      <c r="E33" s="3">
+        <v>41380</v>
+      </c>
+      <c r="F33" s="4">
         <v>5</v>
       </c>
-      <c r="G32" s="38" t="s">
+      <c r="G33" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="39" t="s">
+      <c r="H33" s="36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E33" s="3">
+    <row r="34" spans="5:8">
+      <c r="E34" s="3">
         <v>41381</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F34" s="4">
         <v>3</v>
       </c>
-      <c r="G33" s="38" t="s">
+      <c r="G34" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="39" t="s">
+      <c r="H34" s="36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="3">
+    <row r="35" spans="5:8">
+      <c r="E35" s="3">
         <v>18.0413</v>
       </c>
-      <c r="F34" s="4">
-        <v>2</v>
-      </c>
-      <c r="G34" s="38" t="s">
+      <c r="F35" s="4">
+        <v>2</v>
+      </c>
+      <c r="G35" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="39" t="s">
+      <c r="H35" s="36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="3">
-        <v>41383</v>
-      </c>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8">
       <c r="E36" s="3">
-        <v>41383</v>
+        <v>41382</v>
       </c>
       <c r="F36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" s="39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8">
       <c r="E37" s="3">
         <v>41383</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
       </c>
-      <c r="G37" s="38" t="s">
+      <c r="G37" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8">
+      <c r="E38" s="3">
+        <v>41383</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8">
+      <c r="E39" s="3">
+        <v>41383</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="39" t="s">
+      <c r="H39" s="36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E38" s="3">
+    <row r="40" spans="5:8">
+      <c r="E40" s="3">
         <v>41385</v>
       </c>
-      <c r="F38" s="4">
-        <v>2</v>
-      </c>
-      <c r="G38" s="38" t="s">
+      <c r="F40" s="4">
+        <v>2</v>
+      </c>
+      <c r="G40" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="39" t="s">
+      <c r="H40" s="36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="3">
+    <row r="41" spans="5:8">
+      <c r="E41" s="3">
         <v>41388</v>
       </c>
-      <c r="F39" s="4">
-        <v>2</v>
-      </c>
-      <c r="G39" s="38" t="s">
+      <c r="F41" s="4">
+        <v>2</v>
+      </c>
+      <c r="G41" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="39" t="s">
+      <c r="H41" s="36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E40" s="3">
+    <row r="42" spans="5:8">
+      <c r="E42" s="3">
         <v>40989</v>
       </c>
-      <c r="F40" s="4">
-        <v>2</v>
-      </c>
-      <c r="G40" s="38" t="s">
+      <c r="F42" s="4">
+        <v>2</v>
+      </c>
+      <c r="G42" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="39" t="s">
+      <c r="H42" s="36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E41" s="3">
+    <row r="43" spans="5:8">
+      <c r="E43" s="3">
         <v>41390</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F43" s="4">
         <v>5</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H41" s="6" t="s">
+      <c r="G43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E42" s="3">
+    <row r="44" spans="5:8">
+      <c r="E44" s="3">
         <v>41391</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F44" s="4">
         <v>5</v>
       </c>
-      <c r="G42" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="6" t="s">
+      <c r="G44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E43" s="3">
+    <row r="45" spans="5:8">
+      <c r="E45" s="3">
         <v>41393</v>
       </c>
-      <c r="F43" s="4">
-        <v>1</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H43" s="6" t="s">
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E44" s="3">
+    <row r="46" spans="5:8">
+      <c r="E46" s="3">
         <v>41392</v>
       </c>
-      <c r="F44" s="4">
-        <v>2</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44" s="6" t="s">
+      <c r="F46" s="4">
+        <v>2</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E45" s="3">
-        <v>41390</v>
-      </c>
-      <c r="F45" s="4">
-        <v>2</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E46" s="3">
-        <v>41390</v>
-      </c>
-      <c r="F46" s="4">
-        <v>2</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:8">
       <c r="E47" s="3">
         <v>41390</v>
       </c>
@@ -1847,13 +1913,13 @@
         <v>2</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:8">
       <c r="E48" s="3">
         <v>41390</v>
       </c>
@@ -1861,13 +1927,13 @@
         <v>2</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:8">
       <c r="E49" s="3">
         <v>41390</v>
       </c>
@@ -1875,41 +1941,41 @@
         <v>2</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:8">
       <c r="E50" s="3">
-        <v>41383</v>
+        <v>41390</v>
       </c>
       <c r="F50" s="4">
         <v>2</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:8">
       <c r="E51" s="3">
-        <v>41383</v>
+        <v>41390</v>
       </c>
       <c r="F51" s="4">
         <v>2</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:8">
       <c r="E52" s="3">
         <v>41383</v>
       </c>
@@ -1917,13 +1983,13 @@
         <v>2</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:8">
       <c r="E53" s="3">
         <v>41383</v>
       </c>
@@ -1931,41 +1997,41 @@
         <v>2</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:8">
       <c r="E54" s="3">
-        <v>41393</v>
+        <v>41383</v>
       </c>
       <c r="F54" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="5:8">
       <c r="E55" s="3">
-        <v>41393</v>
+        <v>41383</v>
       </c>
       <c r="F55" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="5:8">
       <c r="E56" s="3">
         <v>41393</v>
       </c>
@@ -1973,13 +2039,13 @@
         <v>1</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:8">
       <c r="E57" s="3">
         <v>41393</v>
       </c>
@@ -1987,13 +2053,13 @@
         <v>1</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:8">
       <c r="E58" s="3">
         <v>41393</v>
       </c>
@@ -2001,83 +2067,83 @@
         <v>1</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:8">
       <c r="E59" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F59" s="4">
+        <v>1</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="5:8">
+      <c r="E60" s="3">
+        <v>41393</v>
+      </c>
+      <c r="F60" s="4">
+        <v>1</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="5:8">
+      <c r="E61" s="3">
         <v>41395</v>
       </c>
-      <c r="F59" s="4">
-        <v>2</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H59" s="4" t="s">
+      <c r="F61" s="4">
+        <v>2</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E60" s="3">
+    <row r="62" spans="5:8">
+      <c r="E62" s="3">
         <v>41396</v>
       </c>
-      <c r="F60" s="4">
-        <v>4</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H60" s="6" t="s">
+      <c r="F62" s="4">
+        <v>4</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E61" s="3">
+    <row r="63" spans="5:8">
+      <c r="E63" s="3">
         <v>41398</v>
       </c>
-      <c r="F61" s="4">
-        <v>2</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H61" s="6" t="s">
+      <c r="F63" s="4">
+        <v>2</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E62" s="3">
-        <v>41397</v>
-      </c>
-      <c r="F62" s="4">
-        <v>1</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="63" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E63" s="3">
-        <v>41397</v>
-      </c>
-      <c r="F63" s="4">
-        <v>1</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:8">
       <c r="E64" s="3">
         <v>41397</v>
       </c>
@@ -2085,97 +2151,97 @@
         <v>1</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:8">
       <c r="E65" s="3">
-        <v>41399</v>
+        <v>41397</v>
       </c>
       <c r="F65" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="5:8">
       <c r="E66" s="3">
-        <v>41399</v>
+        <v>41397</v>
       </c>
       <c r="F66" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8">
       <c r="E67" s="3">
         <v>41399</v>
       </c>
       <c r="F67" s="4">
+        <v>4</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="5:8">
+      <c r="E68" s="3">
+        <v>41399</v>
+      </c>
+      <c r="F68" s="4">
+        <v>7</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="5:8">
+      <c r="E69" s="3">
+        <v>41399</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="5:8">
+      <c r="E70" s="3">
+        <v>41399</v>
+      </c>
+      <c r="F70" s="4">
         <v>3</v>
       </c>
-      <c r="G67" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H67" s="6" t="s">
+      <c r="G70" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H70" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E68" s="3">
-        <v>41400</v>
-      </c>
-      <c r="F68" s="4">
-        <v>1</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E69" s="3">
-        <v>41400</v>
-      </c>
-      <c r="F69" s="4">
-        <v>1</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E70" s="3">
-        <v>41400</v>
-      </c>
-      <c r="F70" s="4">
-        <v>1</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:8">
       <c r="E71" s="3">
         <v>41400</v>
       </c>
@@ -2183,13 +2249,13 @@
         <v>1</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:8">
       <c r="E72" s="3">
         <v>41400</v>
       </c>
@@ -2197,55 +2263,55 @@
         <v>1</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:8">
       <c r="E73" s="3">
-        <v>41407</v>
+        <v>41400</v>
       </c>
       <c r="F73" s="4">
         <v>1</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="5:8">
       <c r="E74" s="3">
-        <v>41407</v>
+        <v>41400</v>
       </c>
       <c r="F74" s="4">
         <v>1</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="5:8">
       <c r="E75" s="3">
-        <v>41407</v>
+        <v>41400</v>
       </c>
       <c r="F75" s="4">
         <v>1</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="5:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="5:8">
       <c r="E76" s="3">
         <v>41407</v>
       </c>
@@ -2253,13 +2319,13 @@
         <v>1</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:8">
       <c r="E77" s="3">
         <v>41407</v>
       </c>
@@ -2267,141 +2333,141 @@
         <v>1</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:8">
       <c r="E78" s="3">
         <v>41407</v>
       </c>
       <c r="F78" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="79" spans="5:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="5:8">
       <c r="E79" s="3">
         <v>41407</v>
       </c>
       <c r="F79" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="5:8">
       <c r="E80" s="3">
-        <v>41402</v>
+        <v>41407</v>
       </c>
       <c r="F80" s="4">
+        <v>1</v>
+      </c>
+      <c r="G80" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G80" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="H80" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="5:8">
       <c r="E81" s="3">
         <v>41407</v>
       </c>
       <c r="F81" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="5:8">
       <c r="E82" s="3">
         <v>41407</v>
       </c>
       <c r="F82" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="5:8">
       <c r="E83" s="3">
-        <v>41408</v>
+        <v>41402</v>
       </c>
       <c r="F83" s="4">
         <v>3</v>
       </c>
       <c r="G83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="5:8">
+      <c r="E84" s="3">
+        <v>41407</v>
+      </c>
+      <c r="F84" s="4">
+        <v>2</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="5:8">
+      <c r="E85" s="3">
+        <v>41407</v>
+      </c>
+      <c r="F85" s="4">
+        <v>1</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="5:8">
+      <c r="E86" s="3">
+        <v>41408</v>
+      </c>
+      <c r="F86" s="4">
         <v>3</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="84" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E84" s="3">
-        <v>41409</v>
-      </c>
-      <c r="F84" s="4">
-        <v>4</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E85" s="3">
-        <v>41410</v>
-      </c>
-      <c r="F85" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E86" s="3">
-        <v>41411</v>
-      </c>
-      <c r="F86" s="4">
-        <v>2</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="5:8">
       <c r="E87" s="3">
-        <v>41412</v>
+        <v>41409</v>
       </c>
       <c r="F87" s="4">
         <v>4</v>
@@ -2410,11 +2476,72 @@
         <v>3</v>
       </c>
       <c r="H87" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="5:8">
+      <c r="E88" s="3">
+        <v>41410</v>
+      </c>
+      <c r="F88" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89" spans="5:8">
+      <c r="E89" s="3">
+        <v>41411</v>
+      </c>
+      <c r="F89" s="4">
+        <v>2</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="5:8">
+      <c r="E90" s="3">
+        <v>41412</v>
+      </c>
+      <c r="F90" s="4">
+        <v>4</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H90" s="6" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="91" spans="5:8">
+      <c r="E91" s="3">
+        <v>41414</v>
+      </c>
+      <c r="F91" s="4">
+        <v>4</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more info in software dev doc and updated arbetsdagbok.
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="64">
   <si>
     <t>Namn</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Mailing, researching documentation, logos</t>
+  </si>
+  <si>
+    <t>Went through rest of lectures (1-4) and identified material to be used in documentation, added in software dev doc</t>
   </si>
 </sst>
 </file>
@@ -466,9 +469,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -566,7 +571,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Följd hyperlänk" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="7" builtinId="9" hidden="1"/>
@@ -575,6 +580,7 @@
     <cellStyle name="Följd hyperlänk" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="6" builtinId="8" hidden="1"/>
@@ -583,6 +589,7 @@
     <cellStyle name="Hyperlänk" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -954,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW92"/>
+  <dimension ref="A1:AW93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1202,7 +1209,7 @@
       </c>
       <c r="C5" s="27">
         <f>SUMIF(G9:G1001,"Sofie",F8:F1001)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="38"/>
@@ -2556,6 +2563,20 @@
         <v>60</v>
       </c>
     </row>
+    <row r="93" spans="5:8">
+      <c r="E93" s="3">
+        <v>41415</v>
+      </c>
+      <c r="F93" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added revised doc, update of arbetsdagbok.
</commit_message>
<xml_diff>
--- a/Arbetsdagbok.xlsx
+++ b/Arbetsdagbok.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19470" windowHeight="6015" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19480" windowHeight="6020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="67">
   <si>
     <t>Namn</t>
   </si>
@@ -218,6 +217,9 @@
   </si>
   <si>
     <t>Most of the time I did refactor</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -476,9 +478,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,25 +584,29 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="20">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+  <cellStyles count="24">
+    <cellStyle name="Följd hyperlänk" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -968,25 +978,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW95"/>
+  <dimension ref="A1:AW97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="1"/>
-    <col min="4" max="4" width="8.875" style="2"/>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
     <col min="5" max="5" width="10.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-    <col min="7" max="7" width="8.875" style="5"/>
-    <col min="8" max="8" width="136.875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.875" style="7"/>
-    <col min="10" max="49" width="8.875" style="1"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="136.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="7"/>
+    <col min="10" max="49" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -1041,13 +1051,13 @@
       <c r="AV1" s="11"/>
       <c r="AW1" s="11"/>
     </row>
-    <row r="2" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="13"/>
       <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="15">
-        <f>SUMIF(G9:G1001,"Fredrik",F9:F1001)</f>
+        <f>SUMIF(G9:G1002,"Fredrik",F9:F1002)</f>
         <v>63</v>
       </c>
       <c r="D2" s="16"/>
@@ -1097,13 +1107,13 @@
       <c r="AV2" s="16"/>
       <c r="AW2" s="16"/>
     </row>
-    <row r="3" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="23">
-        <f>SUMIF(G9:G1001,"Niklas",F9:F1001)</f>
+        <f>SUMIF(G9:G1002,"Niklas",F9:F1002)</f>
         <v>34</v>
       </c>
       <c r="D3" s="16"/>
@@ -1153,13 +1163,13 @@
       <c r="AV3" s="16"/>
       <c r="AW3" s="16"/>
     </row>
-    <row r="4" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="25">
-        <f>SUMIF(G9:G1001,"Anders",F9:F1001)</f>
+        <f>SUMIF(G9:G1002,"Anders",F9:F1002)</f>
         <v>39</v>
       </c>
       <c r="D4" s="16"/>
@@ -1209,14 +1219,14 @@
       <c r="AV4" s="16"/>
       <c r="AW4" s="16"/>
     </row>
-    <row r="5" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="26" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="27">
-        <f>SUMIF(G9:G1001,"Sofie",F8:F1001)</f>
-        <v>29</v>
+        <f>SUMIF(G9:G1002,"Sofie",F8:F1002)</f>
+        <v>41</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="38"/>
@@ -1265,13 +1275,13 @@
       <c r="AV5" s="16"/>
       <c r="AW5" s="16"/>
     </row>
-    <row r="6" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="29">
-        <f>SUMIF(G9:G1001,"Rene",F9:F1001)</f>
+        <f>SUMIF(G9:G1002,"Rene",F9:F1002)</f>
         <v>27</v>
       </c>
       <c r="D6" s="16"/>
@@ -1321,7 +1331,7 @@
       <c r="AV6" s="16"/>
       <c r="AW6" s="16"/>
     </row>
-    <row r="7" spans="1:49" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" s="21" customFormat="1" ht="17.25" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1380,7 +1390,7 @@
       <c r="AV7" s="13"/>
       <c r="AW7" s="13"/>
     </row>
-    <row r="8" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" ht="15" customHeight="1">
       <c r="E8" s="3">
         <v>41352</v>
       </c>
@@ -1394,7 +1404,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" ht="15" customHeight="1">
       <c r="E9" s="3">
         <v>41354</v>
       </c>
@@ -1408,7 +1418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" ht="15" customHeight="1">
       <c r="E10" s="3">
         <v>41354</v>
       </c>
@@ -1422,7 +1432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" ht="15" customHeight="1">
       <c r="E11" s="3">
         <v>41354</v>
       </c>
@@ -1436,7 +1446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" ht="15" customHeight="1">
       <c r="E12" s="3">
         <v>41354</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" ht="15" customHeight="1">
       <c r="E13" s="3">
         <v>41354</v>
       </c>
@@ -1464,7 +1474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" ht="15" customHeight="1">
       <c r="E14" s="3">
         <v>41379</v>
       </c>
@@ -1478,7 +1488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" ht="15" customHeight="1">
       <c r="E15" s="3">
         <v>41379</v>
       </c>
@@ -1492,7 +1502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" ht="15" customHeight="1">
       <c r="E16" s="3">
         <v>41380</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:8" ht="15" customHeight="1">
       <c r="E17" s="3">
         <v>41381</v>
       </c>
@@ -1520,7 +1530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:8" ht="15" customHeight="1">
       <c r="E18" s="3">
         <v>41381</v>
       </c>
@@ -1534,7 +1544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:8" ht="15" customHeight="1">
       <c r="E19" s="3">
         <v>41379</v>
       </c>
@@ -1548,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="5:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:8" ht="15" customHeight="1">
       <c r="E20" s="3">
         <v>41379</v>
       </c>
@@ -1562,7 +1572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:8">
       <c r="E21" s="3">
         <v>41379</v>
       </c>
@@ -1576,7 +1586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:8">
       <c r="E22" s="3">
         <v>41379</v>
       </c>
@@ -1590,7 +1600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:8">
       <c r="E23" s="3">
         <v>41378</v>
       </c>
@@ -1604,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:8">
       <c r="E24" s="3">
         <v>41382</v>
       </c>
@@ -1618,7 +1628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:8">
       <c r="E25" s="3">
         <v>41382</v>
       </c>
@@ -1632,7 +1642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:8">
       <c r="E26" s="3">
         <v>41383</v>
       </c>
@@ -1646,7 +1656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:8">
       <c r="E27" s="3">
         <v>41384</v>
       </c>
@@ -1660,7 +1670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:8">
       <c r="E28" s="3">
         <v>41387</v>
       </c>
@@ -1674,7 +1684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:8">
       <c r="E29" s="3">
         <v>41383</v>
       </c>
@@ -1688,7 +1698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:8">
       <c r="E30" s="3">
         <v>41387</v>
       </c>
@@ -1702,7 +1712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:8">
       <c r="E31" s="3">
         <v>41388</v>
       </c>
@@ -1716,7 +1726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:8">
       <c r="E32" s="3">
         <v>41380</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8">
       <c r="E33" s="3">
         <v>41380</v>
       </c>
@@ -1744,7 +1754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:8">
       <c r="E34" s="3">
         <v>41381</v>
       </c>
@@ -1758,7 +1768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:8">
       <c r="E35" s="3">
         <v>18.0413</v>
       </c>
@@ -1772,7 +1782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8">
       <c r="E36" s="3">
         <v>41382</v>
       </c>
@@ -1786,7 +1796,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:8">
       <c r="E37" s="3">
         <v>41383</v>
       </c>
@@ -1800,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:8">
       <c r="E38" s="3">
         <v>41383</v>
       </c>
@@ -1814,7 +1824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:8">
       <c r="E39" s="3">
         <v>41383</v>
       </c>
@@ -1828,7 +1838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:8">
       <c r="E40" s="3">
         <v>41385</v>
       </c>
@@ -1842,7 +1852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:8">
       <c r="E41" s="3">
         <v>41388</v>
       </c>
@@ -1856,7 +1866,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:8">
       <c r="E42" s="3">
         <v>40989</v>
       </c>
@@ -1870,7 +1880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:8">
       <c r="E43" s="3">
         <v>41390</v>
       </c>
@@ -1884,7 +1894,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:8">
       <c r="E44" s="3">
         <v>41391</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:8">
       <c r="E45" s="3">
         <v>41393</v>
       </c>
@@ -1912,7 +1922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:8">
       <c r="E46" s="3">
         <v>41392</v>
       </c>
@@ -1926,7 +1936,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:8">
       <c r="E47" s="3">
         <v>41390</v>
       </c>
@@ -1940,7 +1950,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:8">
       <c r="E48" s="3">
         <v>41390</v>
       </c>
@@ -1954,7 +1964,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:8">
       <c r="E49" s="3">
         <v>41390</v>
       </c>
@@ -1968,7 +1978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:8">
       <c r="E50" s="3">
         <v>41390</v>
       </c>
@@ -1982,7 +1992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:8">
       <c r="E51" s="3">
         <v>41390</v>
       </c>
@@ -1996,7 +2006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:8">
       <c r="E52" s="3">
         <v>41383</v>
       </c>
@@ -2010,7 +2020,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:8">
       <c r="E53" s="3">
         <v>41383</v>
       </c>
@@ -2024,7 +2034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:8">
       <c r="E54" s="3">
         <v>41383</v>
       </c>
@@ -2038,7 +2048,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:8">
       <c r="E55" s="3">
         <v>41383</v>
       </c>
@@ -2052,7 +2062,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:8">
       <c r="E56" s="3">
         <v>41393</v>
       </c>
@@ -2066,7 +2076,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:8">
       <c r="E57" s="3">
         <v>41393</v>
       </c>
@@ -2080,7 +2090,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:8">
       <c r="E58" s="3">
         <v>41393</v>
       </c>
@@ -2094,7 +2104,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:8">
       <c r="E59" s="3">
         <v>41393</v>
       </c>
@@ -2108,7 +2118,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:8">
       <c r="E60" s="3">
         <v>41393</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:8">
       <c r="E61" s="3">
         <v>41395</v>
       </c>
@@ -2136,7 +2146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:8">
       <c r="E62" s="3">
         <v>41396</v>
       </c>
@@ -2150,7 +2160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:8">
       <c r="E63" s="3">
         <v>41398</v>
       </c>
@@ -2164,7 +2174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:8">
       <c r="E64" s="3">
         <v>41397</v>
       </c>
@@ -2178,7 +2188,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:8">
       <c r="E65" s="3">
         <v>41397</v>
       </c>
@@ -2192,7 +2202,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:8">
       <c r="E66" s="3">
         <v>41397</v>
       </c>
@@ -2206,7 +2216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:8">
       <c r="E67" s="3">
         <v>41399</v>
       </c>
@@ -2220,7 +2230,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:8">
       <c r="E68" s="3">
         <v>41399</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:8">
       <c r="E69" s="3">
         <v>41399</v>
       </c>
@@ -2248,7 +2258,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:8">
       <c r="E70" s="3">
         <v>41399</v>
       </c>
@@ -2262,7 +2272,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:8">
       <c r="E71" s="3">
         <v>41400</v>
       </c>
@@ -2276,7 +2286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:8">
       <c r="E72" s="3">
         <v>41400</v>
       </c>
@@ -2290,7 +2300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:8">
       <c r="E73" s="3">
         <v>41400</v>
       </c>
@@ -2304,7 +2314,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:8">
       <c r="E74" s="3">
         <v>41400</v>
       </c>
@@ -2318,7 +2328,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:8">
       <c r="E75" s="3">
         <v>41400</v>
       </c>
@@ -2332,7 +2342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:8">
       <c r="E76" s="3">
         <v>41407</v>
       </c>
@@ -2346,7 +2356,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:8">
       <c r="E77" s="3">
         <v>41407</v>
       </c>
@@ -2360,7 +2370,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:8">
       <c r="E78" s="3">
         <v>41407</v>
       </c>
@@ -2374,7 +2384,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:8">
       <c r="E79" s="3">
         <v>41407</v>
       </c>
@@ -2388,7 +2398,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:8">
       <c r="E80" s="3">
         <v>41407</v>
       </c>
@@ -2402,7 +2412,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:8">
       <c r="E81" s="3">
         <v>41407</v>
       </c>
@@ -2416,7 +2426,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:8">
       <c r="E82" s="3">
         <v>41407</v>
       </c>
@@ -2430,7 +2440,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:8">
       <c r="E83" s="3">
         <v>41402</v>
       </c>
@@ -2444,7 +2454,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:8">
       <c r="E84" s="3">
         <v>41407</v>
       </c>
@@ -2458,7 +2468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:8">
       <c r="E85" s="3">
         <v>41407</v>
       </c>
@@ -2472,7 +2482,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:8">
       <c r="E86" s="3">
         <v>41408</v>
       </c>
@@ -2486,7 +2496,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:8">
       <c r="E87" s="3">
         <v>41409</v>
       </c>
@@ -2500,7 +2510,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:8">
       <c r="E88" s="3">
         <v>41410</v>
       </c>
@@ -2514,7 +2524,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:8">
       <c r="E89" s="3">
         <v>41411</v>
       </c>
@@ -2528,7 +2538,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:8">
       <c r="E90" s="3">
         <v>41411</v>
       </c>
@@ -2542,7 +2552,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:8">
       <c r="E91" s="3">
         <v>41412</v>
       </c>
@@ -2556,7 +2566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:8">
       <c r="E92" s="3">
         <v>41414</v>
       </c>
@@ -2570,7 +2580,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:8">
       <c r="E93" s="3">
         <v>41415</v>
       </c>
@@ -2584,7 +2594,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="94" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:8">
       <c r="E94" s="3">
         <v>41416</v>
       </c>
@@ -2598,18 +2608,46 @@
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:8">
       <c r="E95" s="3">
+        <v>41416</v>
+      </c>
+      <c r="F95" s="4">
+        <v>5</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="5:8">
+      <c r="E96" s="3">
         <v>41417</v>
       </c>
-      <c r="F95" s="4">
+      <c r="F96" s="4">
         <v>6</v>
       </c>
-      <c r="G95" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H95" s="6" t="s">
+      <c r="G96" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H96" s="6" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="97" spans="5:8">
+      <c r="E97" s="3">
+        <v>41417</v>
+      </c>
+      <c r="F97" s="4">
+        <v>7</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>